<commit_message>
Modify code so that it can deal with nonconsecutive bus numbers
Modified large-scale case so that its LTCs and phase shifters are all
fixed tap transformers with tap ratio = 1.0. Creates undervoltage
issues. Have not partitioned yet. Currently trying to deal with existing
area numbers. Some are very small, and others are very large. See if the
solutions can still reconcile. If not, partition into smaller sizes.

Fixing issue where code can't deal with bus numbers that don't equal the
bus index number (i.e. buses(24) != bus 24).
</commit_message>
<xml_diff>
--- a/DMASE - Partition Results.xlsx
+++ b/DMASE - Partition Results.xlsx
@@ -1576,7 +1576,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>D-MASE</a:t>
+              <a:t>118 Bus D-MASE</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -1605,10 +1605,10 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>'Timing New'!$L$16:$L$21</c:f>
+              <c:f>'Timing New'!$L$16:$L$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1622,9 +1622,12 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
@@ -1632,10 +1635,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Timing New'!$M$16:$M$21</c:f>
+              <c:f>'Timing New'!$M$16:$M$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>10.388287607637281</c:v>
                 </c:pt>
@@ -1648,10 +1651,10 @@
                 <c:pt idx="3">
                   <c:v>3.1007822210910057</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>3.1658189862136719</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>3.3424936213691523</c:v>
                 </c:pt>
               </c:numCache>
@@ -8955,8 +8958,8 @@
   </sheetPr>
   <dimension ref="A1:V44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9874,11 +9877,9 @@
     <row r="20" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
       <c r="L20">
-        <v>16</v>
-      </c>
-      <c r="M20" s="4">
-        <v>3.1658189862136719</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="M20" s="4"/>
       <c r="N20" s="4"/>
       <c r="Q20">
         <v>0.37099963394088398</v>
@@ -9903,16 +9904,21 @@
     <row r="21" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
       <c r="L21">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="M21" s="4">
-        <v>3.3424936213691523</v>
+        <v>3.1658189862136719</v>
       </c>
       <c r="N21" s="4"/>
     </row>
     <row r="22" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B22" s="5"/>
-      <c r="M22" s="4"/>
+      <c r="L22">
+        <v>32</v>
+      </c>
+      <c r="M22" s="4">
+        <v>3.3424936213691523</v>
+      </c>
       <c r="N22" s="4"/>
     </row>
     <row r="23" spans="2:22" x14ac:dyDescent="0.25">
@@ -9932,15 +9938,16 @@
     </row>
     <row r="26" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
+      <c r="M26" s="4"/>
       <c r="N26" s="4"/>
     </row>
     <row r="27" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
-      <c r="M27" s="4"/>
       <c r="N27" s="4"/>
     </row>
     <row r="28" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B28" s="5"/>
+      <c r="M28" s="4"/>
       <c r="N28" s="4"/>
     </row>
     <row r="29" spans="2:22" x14ac:dyDescent="0.25">
@@ -9995,7 +10002,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="40" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup scale="57" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Lots of changes due to revert; prelim data for GM 2016
A lot of changes in this commit, because I freaked out and reverted to
an older version when I thought the 14 bus system wasn't working. It is
now, and I have some preliminary data for that plus the 118. Next time,
try to get the 57 bus system working and see if can draw a trend from
the number of partitions vs computational speed.
</commit_message>
<xml_diff>
--- a/DMASE - Partition Results.xlsx
+++ b/DMASE - Partition Results.xlsx
@@ -1514,6 +1514,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1532,11 +1537,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1670,11 +1670,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="80775040"/>
-        <c:axId val="80773504"/>
+        <c:axId val="199259648"/>
+        <c:axId val="199261568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80775040"/>
+        <c:axId val="199259648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1703,12 +1703,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80773504"/>
+        <c:crossAx val="199261568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80773504"/>
+        <c:axId val="199261568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1738,7 +1738,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80775040"/>
+        <c:crossAx val="199259648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3704,31 +3704,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="24" t="s">
         <v>397</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="I1" s="21" t="s">
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="I1" s="24" t="s">
         <v>395</v>
       </c>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="O1" s="21" t="s">
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="O1" s="24" t="s">
         <v>395</v>
       </c>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="U1" s="21" t="s">
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="U1" s="24" t="s">
         <v>395</v>
       </c>
-      <c r="V1" s="21"/>
-      <c r="W1" s="21"/>
-      <c r="AA1" s="23" t="s">
+      <c r="V1" s="24"/>
+      <c r="W1" s="24"/>
+      <c r="AA1" s="26" t="s">
         <v>395</v>
       </c>
-      <c r="AB1" s="23"/>
-      <c r="AC1" s="23"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -6176,7 +6176,7 @@
       <c r="R7" s="3">
         <v>-0.03</v>
       </c>
-      <c r="S7" s="24">
+      <c r="S7" s="18">
         <v>-0.03</v>
       </c>
       <c r="T7">
@@ -8958,8 +8958,8 @@
   </sheetPr>
   <dimension ref="A1:V44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9426,7 +9426,7 @@
         <v>10.608314551928601</v>
       </c>
       <c r="M9" s="4">
-        <f>AVERAGE(C9:L9)</f>
+        <f t="shared" ref="M9:M14" si="1">AVERAGE(C9:L9)</f>
         <v>10.388287607637281</v>
       </c>
       <c r="N9" s="4"/>
@@ -9484,7 +9484,7 @@
         <v>4.1173247526714896</v>
       </c>
       <c r="M10" s="4">
-        <f>AVERAGE(C10:L10)</f>
+        <f t="shared" si="1"/>
         <v>4.130446794886562</v>
       </c>
       <c r="N10" s="4"/>
@@ -9542,7 +9542,7 @@
         <v>3.3170763727906998</v>
       </c>
       <c r="M11" s="4">
-        <f>AVERAGE(C11:L11)</f>
+        <f t="shared" si="1"/>
         <v>3.3559261384352128</v>
       </c>
       <c r="N11" s="4"/>
@@ -9600,7 +9600,7 @@
         <v>3.0589207396834799</v>
       </c>
       <c r="M12" s="4">
-        <f>AVERAGE(C12:L12)</f>
+        <f t="shared" si="1"/>
         <v>3.1007822210910057</v>
       </c>
       <c r="N12" s="4"/>
@@ -9627,38 +9627,38 @@
       <c r="B13" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="25">
+      <c r="C13" s="19">
         <v>3.3029027752941</v>
       </c>
-      <c r="D13" s="26">
+      <c r="D13" s="20">
         <v>3.1535223170712499</v>
       </c>
-      <c r="E13" s="26">
+      <c r="E13" s="20">
         <v>3.1493570537582301</v>
       </c>
-      <c r="F13" s="26">
+      <c r="F13" s="20">
         <v>3.1473603603702398</v>
       </c>
-      <c r="G13" s="26">
+      <c r="G13" s="20">
         <v>3.1371311465518099</v>
       </c>
-      <c r="H13" s="26">
+      <c r="H13" s="20">
         <v>3.1603981099432001</v>
       </c>
-      <c r="I13" s="26">
+      <c r="I13" s="20">
         <v>3.14894125881644</v>
       </c>
-      <c r="J13" s="26">
+      <c r="J13" s="20">
         <v>3.1418738418904102</v>
       </c>
-      <c r="K13" s="26">
+      <c r="K13" s="20">
         <v>3.1607996427893599</v>
       </c>
-      <c r="L13" s="26">
+      <c r="L13" s="20">
         <v>3.15590335565168</v>
       </c>
       <c r="M13" s="4">
-        <f>AVERAGE(C13:L13)</f>
+        <f t="shared" si="1"/>
         <v>3.1658189862136719</v>
       </c>
       <c r="N13" s="4"/>
@@ -9701,7 +9701,7 @@
         <v>3.3330985572976002</v>
       </c>
       <c r="M14" s="4">
-        <f>AVERAGE(C14:L14)</f>
+        <f t="shared" si="1"/>
         <v>3.3424936213691523</v>
       </c>
       <c r="N14" s="4"/>
@@ -9721,7 +9721,7 @@
         <v>0.36839041137218798</v>
       </c>
       <c r="V14">
-        <f t="shared" ref="V14:V20" si="1">SUM(Q14:U14)</f>
+        <f t="shared" ref="V14:V20" si="2">SUM(Q14:U14)</f>
         <v>1.846933532660628</v>
       </c>
     </row>
@@ -9748,7 +9748,7 @@
         <v>0.62008622319512896</v>
       </c>
       <c r="V15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.2097237149624558</v>
       </c>
     </row>
@@ -9777,7 +9777,7 @@
         <v>0.36710207344513601</v>
       </c>
       <c r="V16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.835220006648308</v>
       </c>
     </row>
@@ -9809,7 +9809,7 @@
         <v>0.61966896700019103</v>
       </c>
       <c r="V17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.1991134860054609</v>
       </c>
     </row>
@@ -9838,7 +9838,7 @@
         <v>0.36731234716300498</v>
       </c>
       <c r="V18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.8344257205348931</v>
       </c>
     </row>
@@ -9870,7 +9870,7 @@
         <v>0.62270056547173902</v>
       </c>
       <c r="V19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.2174884833998956</v>
       </c>
     </row>
@@ -9897,7 +9897,7 @@
         <v>0.36932878069401998</v>
       </c>
       <c r="V20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.8517087573700939</v>
       </c>
     </row>
@@ -11313,44 +11313,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33 16384:16384" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="D1" s="18" t="s">
+      <c r="B1" s="22"/>
+      <c r="D1" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="19"/>
-      <c r="I1" s="18" t="s">
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="22"/>
+      <c r="I1" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="19"/>
-      <c r="R1" s="18" t="s">
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="22"/>
+      <c r="R1" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="S1" s="20"/>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
-      <c r="V1" s="20"/>
-      <c r="W1" s="20"/>
-      <c r="X1" s="20"/>
-      <c r="Y1" s="20"/>
-      <c r="Z1" s="20"/>
-      <c r="AA1" s="20"/>
-      <c r="AB1" s="20"/>
-      <c r="AC1" s="20"/>
-      <c r="AD1" s="20"/>
-      <c r="AE1" s="20"/>
-      <c r="AF1" s="20"/>
-      <c r="AG1" s="19"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
+      <c r="V1" s="23"/>
+      <c r="W1" s="23"/>
+      <c r="X1" s="23"/>
+      <c r="Y1" s="23"/>
+      <c r="Z1" s="23"/>
+      <c r="AA1" s="23"/>
+      <c r="AB1" s="23"/>
+      <c r="AC1" s="23"/>
+      <c r="AD1" s="23"/>
+      <c r="AE1" s="23"/>
+      <c r="AF1" s="23"/>
+      <c r="AG1" s="22"/>
       <c r="XFD1" t="s">
         <v>10</v>
       </c>
@@ -13646,26 +13646,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="24" t="s">
         <v>287</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
       <c r="H1" s="9"/>
-      <c r="K1" s="21" t="s">
+      <c r="K1" s="24" t="s">
         <v>288</v>
       </c>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -15397,16 +15397,16 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J33" s="21" t="s">
+      <c r="J33" s="24" t="s">
         <v>297</v>
       </c>
-      <c r="K33" s="21"/>
-      <c r="L33" s="21"/>
-      <c r="M33" s="21"/>
-      <c r="N33" s="21"/>
-      <c r="O33" s="21"/>
-      <c r="P33" s="21"/>
-      <c r="Q33" s="21"/>
+      <c r="K33" s="24"/>
+      <c r="L33" s="24"/>
+      <c r="M33" s="24"/>
+      <c r="N33" s="24"/>
+      <c r="O33" s="24"/>
+      <c r="P33" s="24"/>
+      <c r="Q33" s="24"/>
       <c r="R33" s="7"/>
       <c r="S33" s="7"/>
       <c r="T33" s="7"/>
@@ -16871,16 +16871,16 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="J65" s="21" t="s">
+      <c r="J65" s="24" t="s">
         <v>298</v>
       </c>
-      <c r="K65" s="21"/>
-      <c r="L65" s="21"/>
-      <c r="M65" s="21"/>
-      <c r="N65" s="21"/>
-      <c r="O65" s="21"/>
-      <c r="P65" s="21"/>
-      <c r="Q65" s="21"/>
+      <c r="K65" s="24"/>
+      <c r="L65" s="24"/>
+      <c r="M65" s="24"/>
+      <c r="N65" s="24"/>
+      <c r="O65" s="24"/>
+      <c r="P65" s="24"/>
+      <c r="Q65" s="24"/>
       <c r="R65" s="7"/>
       <c r="S65" s="7"/>
       <c r="T65" s="7"/>
@@ -18366,19 +18366,19 @@
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="K98" s="21" t="s">
+      <c r="K98" s="24" t="s">
         <v>299</v>
       </c>
-      <c r="L98" s="21"/>
-      <c r="M98" s="21"/>
-      <c r="N98" s="21"/>
-      <c r="O98" s="21"/>
-      <c r="P98" s="21"/>
-      <c r="Q98" s="21"/>
-      <c r="R98" s="21"/>
-      <c r="S98" s="21"/>
-      <c r="T98" s="21"/>
-      <c r="U98" s="21"/>
+      <c r="L98" s="24"/>
+      <c r="M98" s="24"/>
+      <c r="N98" s="24"/>
+      <c r="O98" s="24"/>
+      <c r="P98" s="24"/>
+      <c r="Q98" s="24"/>
+      <c r="R98" s="24"/>
+      <c r="S98" s="24"/>
+      <c r="T98" s="24"/>
+      <c r="U98" s="24"/>
     </row>
     <row r="99" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A99">
@@ -19853,59 +19853,59 @@
       <c r="D1" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="1"/>
-      <c r="L1" s="21" t="s">
+      <c r="L1" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
       <c r="P1" s="7"/>
-      <c r="Q1" s="21" t="s">
+      <c r="Q1" s="24" t="s">
         <v>354</v>
       </c>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
-      <c r="T1" s="21"/>
-      <c r="U1" s="21"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="24"/>
+      <c r="U1" s="24"/>
       <c r="V1" s="7"/>
-      <c r="W1" s="21" t="s">
+      <c r="W1" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="X1" s="21"/>
-      <c r="Y1" s="21"/>
-      <c r="Z1" s="21"/>
-      <c r="AA1" s="21"/>
-      <c r="AB1" s="21"/>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="24"/>
+      <c r="Z1" s="24"/>
+      <c r="AA1" s="24"/>
+      <c r="AB1" s="24"/>
       <c r="AC1" s="10"/>
       <c r="AD1" s="10" t="s">
         <v>356</v>
       </c>
-      <c r="AF1" s="21" t="s">
+      <c r="AF1" s="24" t="s">
         <v>355</v>
       </c>
-      <c r="AG1" s="21"/>
-      <c r="AH1" s="21"/>
-      <c r="AI1" s="21"/>
-      <c r="AJ1" s="21"/>
-      <c r="AK1" s="21"/>
-      <c r="AL1" s="21"/>
-      <c r="AM1" s="21"/>
+      <c r="AG1" s="24"/>
+      <c r="AH1" s="24"/>
+      <c r="AI1" s="24"/>
+      <c r="AJ1" s="24"/>
+      <c r="AK1" s="24"/>
+      <c r="AL1" s="24"/>
+      <c r="AM1" s="24"/>
       <c r="AN1" s="10"/>
-      <c r="AO1" s="23"/>
-      <c r="AP1" s="23"/>
-      <c r="AQ1" s="23"/>
-      <c r="AR1" s="23"/>
-      <c r="AS1" s="23"/>
-      <c r="AT1" s="23"/>
+      <c r="AO1" s="26"/>
+      <c r="AP1" s="26"/>
+      <c r="AQ1" s="26"/>
+      <c r="AR1" s="26"/>
+      <c r="AS1" s="26"/>
+      <c r="AT1" s="26"/>
       <c r="AU1" s="2"/>
       <c r="AV1" s="2"/>
     </row>
@@ -20080,7 +20080,7 @@
         <v>-4.6651244400841563E-6</v>
       </c>
       <c r="AC3" s="8"/>
-      <c r="AD3" s="22" t="s">
+      <c r="AD3" s="25" t="s">
         <v>357</v>
       </c>
       <c r="AF3" s="2"/>
@@ -20186,7 +20186,7 @@
         <v>-4.9801974499885659E-6</v>
       </c>
       <c r="AC4" s="8"/>
-      <c r="AD4" s="22"/>
+      <c r="AD4" s="25"/>
       <c r="AF4" s="2"/>
       <c r="AG4" s="2"/>
       <c r="AH4" s="2"/>
@@ -20288,7 +20288,7 @@
         <v>-5.0402674698357686E-6</v>
       </c>
       <c r="AC5" s="8"/>
-      <c r="AD5" s="22"/>
+      <c r="AD5" s="25"/>
       <c r="AF5" s="2"/>
       <c r="AG5" s="2"/>
       <c r="AH5" s="2"/>
@@ -20398,7 +20398,7 @@
         <v>3.2983009832232568E-6</v>
       </c>
       <c r="AC6" s="8"/>
-      <c r="AD6" s="22"/>
+      <c r="AD6" s="25"/>
       <c r="AF6" s="2"/>
       <c r="AG6" s="2"/>
       <c r="AH6" s="2">
@@ -20512,7 +20512,7 @@
         <v>-9.0380602335571325E-7</v>
       </c>
       <c r="AC7" s="8"/>
-      <c r="AD7" s="22"/>
+      <c r="AD7" s="25"/>
       <c r="AF7" s="2"/>
       <c r="AG7" s="2">
         <v>1.0247001050681701</v>
@@ -20622,7 +20622,7 @@
         <v>5.3391086698439949E-6</v>
       </c>
       <c r="AC8" s="8"/>
-      <c r="AD8" s="22"/>
+      <c r="AD8" s="25"/>
       <c r="AF8" s="2">
         <v>1.01684788547473</v>
       </c>
@@ -20732,7 +20732,7 @@
         <v>1.2067012249428188E-6</v>
       </c>
       <c r="AC9" s="8"/>
-      <c r="AD9" s="22"/>
+      <c r="AD9" s="25"/>
       <c r="AF9" s="2"/>
       <c r="AG9" s="2"/>
       <c r="AH9" s="2">
@@ -20832,7 +20832,7 @@
         <v>-3.4640150698983518E-6</v>
       </c>
       <c r="AC10" s="8"/>
-      <c r="AD10" s="22"/>
+      <c r="AD10" s="25"/>
       <c r="AF10" s="2"/>
       <c r="AG10" s="2"/>
       <c r="AH10" s="2"/>
@@ -20938,7 +20938,7 @@
         <v>1.7235567049134204E-6</v>
       </c>
       <c r="AC11" s="8"/>
-      <c r="AD11" s="22"/>
+      <c r="AD11" s="25"/>
       <c r="AF11" s="2">
         <v>1.0122489616983801</v>
       </c>
@@ -21044,7 +21044,7 @@
         <v>3.6109064749378916E-6</v>
       </c>
       <c r="AC12" s="8"/>
-      <c r="AD12" s="22"/>
+      <c r="AD12" s="25"/>
       <c r="AF12" s="2">
         <v>1.0045090763897699</v>
       </c>
@@ -21148,7 +21148,7 @@
         <v>3.5827228299645242E-6</v>
       </c>
       <c r="AC13" s="8"/>
-      <c r="AD13" s="22"/>
+      <c r="AD13" s="25"/>
       <c r="AF13" s="2">
         <v>1.0067034208641199</v>
       </c>
@@ -21248,7 +21248,7 @@
         <v>8.1732388165223213E-6</v>
       </c>
       <c r="AC14" s="8"/>
-      <c r="AD14" s="22"/>
+      <c r="AD14" s="25"/>
       <c r="AF14" s="2"/>
       <c r="AG14" s="2">
         <v>0.99918593137599498</v>
@@ -21350,7 +21350,7 @@
         <v>8.4509885035499721E-6</v>
       </c>
       <c r="AC15" s="8"/>
-      <c r="AD15" s="22"/>
+      <c r="AD15" s="25"/>
       <c r="AF15" s="2"/>
       <c r="AG15" s="2">
         <v>0.99501225501224599</v>
@@ -21452,7 +21452,7 @@
         <v>3.5116233489951298E-6</v>
       </c>
       <c r="AC16" s="8"/>
-      <c r="AD16" s="22"/>
+      <c r="AD16" s="25"/>
       <c r="AF16" s="2"/>
       <c r="AG16" s="2"/>
       <c r="AH16" s="2">
@@ -21548,7 +21548,7 @@
         <v>0</v>
       </c>
       <c r="AC17" s="8"/>
-      <c r="AD17" s="22"/>
+      <c r="AD17" s="25"/>
       <c r="AF17" s="2"/>
       <c r="AG17" s="2"/>
       <c r="AH17" s="2"/>
@@ -21650,7 +21650,7 @@
         <v>-1.6353210543079699E-6</v>
       </c>
       <c r="AC18" s="8"/>
-      <c r="AD18" s="22"/>
+      <c r="AD18" s="25"/>
       <c r="AF18" s="2"/>
       <c r="AG18" s="2"/>
       <c r="AH18" s="2"/>
@@ -21752,7 +21752,7 @@
         <v>-1.6203253555002739E-6</v>
       </c>
       <c r="AC19" s="8"/>
-      <c r="AD19" s="22"/>
+      <c r="AD19" s="25"/>
       <c r="AF19" s="2"/>
       <c r="AG19" s="2"/>
       <c r="AH19" s="2"/>
@@ -21862,7 +21862,7 @@
         <v>-4.3676463393482745E-6</v>
       </c>
       <c r="AC20" s="8"/>
-      <c r="AD20" s="22"/>
+      <c r="AD20" s="25"/>
       <c r="AF20" s="2"/>
       <c r="AG20" s="2"/>
       <c r="AH20" s="2">
@@ -21976,7 +21976,7 @@
         <v>-2.5495926090080001E-6</v>
       </c>
       <c r="AC21" s="8"/>
-      <c r="AD21" s="22"/>
+      <c r="AD21" s="25"/>
       <c r="AF21" s="2"/>
       <c r="AG21" s="2">
         <v>-0.13805167133004501</v>
@@ -22086,7 +22086,7 @@
         <v>-2.9561231789931863E-6</v>
       </c>
       <c r="AC22" s="8"/>
-      <c r="AD22" s="22"/>
+      <c r="AD22" s="25"/>
       <c r="AF22" s="2">
         <v>-0.23811107459262901</v>
       </c>
@@ -22196,7 +22196,7 @@
         <v>2.0343429495139898E-6</v>
       </c>
       <c r="AC23" s="8"/>
-      <c r="AD23" s="22"/>
+      <c r="AD23" s="25"/>
       <c r="AF23" s="2"/>
       <c r="AG23" s="2"/>
       <c r="AH23" s="2">
@@ -22296,7 +22296,7 @@
         <v>-4.3863299997726202E-7</v>
       </c>
       <c r="AC24" s="8"/>
-      <c r="AD24" s="22"/>
+      <c r="AD24" s="25"/>
       <c r="AF24" s="2"/>
       <c r="AG24" s="2"/>
       <c r="AH24" s="2"/>
@@ -22402,7 +22402,7 @@
         <v>1.2238704490130647E-6</v>
       </c>
       <c r="AC25" s="8"/>
-      <c r="AD25" s="22"/>
+      <c r="AD25" s="25"/>
       <c r="AF25" s="2">
         <v>-0.246662433797529</v>
       </c>
@@ -22508,7 +22508,7 @@
         <v>1.6678690910043592E-6</v>
       </c>
       <c r="AC26" s="8"/>
-      <c r="AD26" s="22"/>
+      <c r="AD26" s="25"/>
       <c r="AF26" s="2">
         <v>-0.248682381662202</v>
       </c>
@@ -22612,7 +22612,7 @@
         <v>2.4757774094996687E-6</v>
       </c>
       <c r="AC27" s="8"/>
-      <c r="AD27" s="22"/>
+      <c r="AD27" s="25"/>
       <c r="AF27" s="2">
         <v>-0.245119490275858</v>
       </c>
@@ -22712,7 +22712,7 @@
         <v>-4.8735033979507847E-6</v>
       </c>
       <c r="AC28" s="8"/>
-      <c r="AD28" s="22"/>
+      <c r="AD28" s="25"/>
       <c r="AF28" s="2"/>
       <c r="AG28" s="2">
         <v>-0.25008120992174898</v>
@@ -22814,7 +22814,7 @@
         <v>-3.2348925199654488E-6</v>
       </c>
       <c r="AC29" s="8"/>
-      <c r="AD29" s="22"/>
+      <c r="AD29" s="25"/>
       <c r="AF29" s="2"/>
       <c r="AG29" s="2">
         <v>-0.25047172796811701</v>
@@ -22916,7 +22916,7 @@
         <v>7.7221535250138196E-6</v>
       </c>
       <c r="AC30" s="8"/>
-      <c r="AD30" s="22"/>
+      <c r="AD30" s="25"/>
       <c r="AF30" s="2"/>
       <c r="AG30" s="2"/>
       <c r="AH30" s="2">
@@ -23213,44 +23213,44 @@
       <c r="C1" t="s">
         <v>61</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="24" t="s">
         <v>276</v>
       </c>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
       <c r="I1" s="6"/>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
       <c r="N1" s="7"/>
-      <c r="O1" s="21" t="s">
+      <c r="O1" s="24" t="s">
         <v>354</v>
       </c>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
       <c r="T1" s="10"/>
-      <c r="U1" s="21" t="s">
+      <c r="U1" s="24" t="s">
         <v>307</v>
       </c>
-      <c r="V1" s="21"/>
-      <c r="W1" s="21"/>
-      <c r="X1" s="21"/>
-      <c r="Y1" s="21"/>
-      <c r="Z1" s="21"/>
-      <c r="AB1" s="21" t="s">
+      <c r="V1" s="24"/>
+      <c r="W1" s="24"/>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="24"/>
+      <c r="Z1" s="24"/>
+      <c r="AB1" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="AC1" s="21"/>
-      <c r="AD1" s="21"/>
-      <c r="AE1" s="21"/>
-      <c r="AF1" s="21"/>
-      <c r="AG1" s="21"/>
+      <c r="AC1" s="24"/>
+      <c r="AD1" s="24"/>
+      <c r="AE1" s="24"/>
+      <c r="AF1" s="24"/>
+      <c r="AG1" s="24"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="E2" t="s">
@@ -41638,41 +41638,41 @@
       <c r="C1" t="s">
         <v>61</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="24" t="s">
         <v>409</v>
       </c>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
       <c r="I1" s="7"/>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="24" t="s">
         <v>410</v>
       </c>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
       <c r="O1" s="15"/>
-      <c r="P1" s="21" t="s">
+      <c r="P1" s="24" t="s">
         <v>411</v>
       </c>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
-      <c r="T1" s="21"/>
-      <c r="U1" s="21"/>
-      <c r="W1" s="21" t="s">
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="24"/>
+      <c r="U1" s="24"/>
+      <c r="W1" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="X1" s="21"/>
-      <c r="Y1" s="21"/>
-      <c r="Z1" s="21"/>
-      <c r="AA1" s="21"/>
-      <c r="AB1" s="21"/>
-      <c r="AC1" s="21"/>
-      <c r="AD1" s="21"/>
-      <c r="AE1" s="21"/>
-      <c r="AF1" s="21"/>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="24"/>
+      <c r="Z1" s="24"/>
+      <c r="AA1" s="24"/>
+      <c r="AB1" s="24"/>
+      <c r="AC1" s="24"/>
+      <c r="AD1" s="24"/>
+      <c r="AE1" s="24"/>
+      <c r="AF1" s="24"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="E2" t="s">

</xml_diff>

<commit_message>
Fixed central SE; tried running on IEEE 57 and 300 cases; issues/get ill-conditioned Gain
Fixed the central SE code so that it only uses 2*numlines+3*numbus
measurements. Got central times for 14, 57, and 118. DMASE doesn't work
on 57 and 300 cases. Get error saying ill-conditioned or close to
singular Gain. Maybe it's the way I set up an extra padded row/column
for the slack. Check that.

Also, IEEE 300 case has DC line. How to treat? Just ignore and compare
against the same central?
</commit_message>
<xml_diff>
--- a/DMASE - Partition Results.xlsx
+++ b/DMASE - Partition Results.xlsx
@@ -1670,11 +1670,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="199259648"/>
-        <c:axId val="199261568"/>
+        <c:axId val="233059456"/>
+        <c:axId val="233061376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="199259648"/>
+        <c:axId val="233059456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1703,12 +1703,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="199261568"/>
+        <c:crossAx val="233061376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="199261568"/>
+        <c:axId val="233061376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1738,7 +1738,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="199259648"/>
+        <c:crossAx val="233059456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>

</xml_diff>